<commit_message>
🔥 [add] concepto baja y direcciones
</commit_message>
<xml_diff>
--- a/formatos/EstructuraOrganizacional.xlsx
+++ b/formatos/EstructuraOrganizacional.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eperez\Desktop\Sistema Amaxonia\Info Sist RH\2025-02-28\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eperez\Desktop\Sistema Amaxonia\Info Sist RH\2025-03-12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B27BF31-2936-4826-A9B6-A9A9AFF706CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDFC7F0C-77E7-45D6-A48C-5515DC2E6551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F3A26CC-552D-47EF-8EB8-849130DBF44D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E5D0CDA1-6DB2-4E9F-9A7B-8F72B0CF3A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="207">
   <si>
     <t>VP</t>
   </si>
@@ -65,9 +65,24 @@
     <t>000-01 Sec Relaciones Públicas y Comunicación</t>
   </si>
   <si>
+    <t>000-02 Sec Salón Diplomatico</t>
+  </si>
+  <si>
     <t>001 Dep de Auditoria</t>
   </si>
   <si>
+    <t>002 Dep de Desarrollo Organizacional</t>
+  </si>
+  <si>
+    <t>002-01 Secc Procesos</t>
+  </si>
+  <si>
+    <t>003 Dep de Planificacion y Estrategia</t>
+  </si>
+  <si>
+    <t>003-01 Gestion Integral</t>
+  </si>
+  <si>
     <t>010 VP Legal</t>
   </si>
   <si>
@@ -275,6 +290,15 @@
     <t>104-00-02 Eq Coordinadores de Terminal</t>
   </si>
   <si>
+    <t>104-01 Sec Coordinacion de Servicios y Apoyo</t>
+  </si>
+  <si>
+    <t>104-02 Sec Imagen Visual y Contenido</t>
+  </si>
+  <si>
+    <t>104-03 Sec Servicio al Pasajero</t>
+  </si>
+  <si>
     <t>200 VP Finanzas y Administración</t>
   </si>
   <si>
@@ -329,6 +353,18 @@
     <t>202-04 Sec Bienes Patrimoniales</t>
   </si>
   <si>
+    <t>203 Dep de Planificacion de Inversiones</t>
+  </si>
+  <si>
+    <t>203-01 Sección de Planificación de Inversiones de Capital</t>
+  </si>
+  <si>
+    <t>204 Dep de Centro de Excelencia de Procesos</t>
+  </si>
+  <si>
+    <t>204-01 Sección de Procesos</t>
+  </si>
+  <si>
     <t>300 VP Ingeniería y Administración de Proyecto</t>
   </si>
   <si>
@@ -368,6 +404,9 @@
     <t>400-00-03 Eq Compensación y Estructura</t>
   </si>
   <si>
+    <t>400-01 Sec de Relaciones Laborales</t>
+  </si>
+  <si>
     <t>401 Dep de Desarrollo de Recursos Humanos</t>
   </si>
   <si>
@@ -455,6 +494,15 @@
     <t>703­01­02­01 Soporte Técnico</t>
   </si>
   <si>
+    <t>704 Dep Zona Logistica y Carga</t>
+  </si>
+  <si>
+    <t>704-01  Operaciones Carga Tocumen</t>
+  </si>
+  <si>
+    <t>704-02  Estrategia e Inteligencia de Negocios Aeroportuarios</t>
+  </si>
+  <si>
     <t>705 Dep Experiencia del Pasajero</t>
   </si>
   <si>
@@ -462,6 +510,15 @@
   </si>
   <si>
     <t>705-00-01 Coordinadores de Terminal</t>
+  </si>
+  <si>
+    <t>705-01 Servicio al Pasajero</t>
+  </si>
+  <si>
+    <t>705-02 Coordinacion de Servicios y Apoyo</t>
+  </si>
+  <si>
+    <t>705-03 Imagen Visual y Contenido</t>
   </si>
   <si>
     <t>800 VP Tecnología</t>
@@ -606,8 +663,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -635,8 +700,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,10 +1036,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0413EB94-04B1-4BF3-AEB4-2BCEDEF04092}">
-  <dimension ref="A1:E135"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1711A78B-1D92-41B1-B3E3-CE49DC1666ED}">
+  <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -981,22 +1049,23 @@
     <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1044,7 +1113,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -1052,7 +1121,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -1060,27 +1129,21 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1088,331 +1151,319 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
         <v>26</v>
       </c>
-      <c r="D17" t="s">
-        <v>27</v>
+      <c r="E17" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="D18" t="s">
-        <v>28</v>
+      <c r="E18" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
-        <v>29</v>
+      <c r="E19" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
         <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C30" t="s">
         <v>43</v>
@@ -1420,408 +1471,417 @@
       <c r="D30" t="s">
         <v>44</v>
       </c>
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
         <v>43</v>
       </c>
-      <c r="C31" t="s">
-        <v>45</v>
-      </c>
       <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
         <v>43</v>
       </c>
-      <c r="C32" t="s">
-        <v>45</v>
-      </c>
       <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
         <v>48</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D39" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" t="s">
         <v>51</v>
-      </c>
-      <c r="D40" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C44" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D44" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D45" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D46" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C47" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D47" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C48" t="s">
         <v>62</v>
       </c>
       <c r="D48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
         <v>62</v>
       </c>
       <c r="D49" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s">
         <v>62</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C52" t="s">
         <v>67</v>
       </c>
       <c r="D52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C53" t="s">
         <v>67</v>
       </c>
       <c r="D53" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C54" t="s">
         <v>67</v>
       </c>
       <c r="D54" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D55" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C56" t="s">
         <v>72</v>
       </c>
       <c r="D56" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C57" t="s">
         <v>72</v>
       </c>
       <c r="D57" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C58" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58" t="s">
         <v>76</v>
-      </c>
-      <c r="D58" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D59" t="s">
         <v>78</v>
@@ -1829,132 +1889,132 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" t="s">
         <v>79</v>
-      </c>
-      <c r="B60" t="s">
-        <v>79</v>
-      </c>
-      <c r="C60" t="s">
-        <v>80</v>
-      </c>
-      <c r="D60" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" t="s">
         <v>82</v>
-      </c>
-      <c r="C61" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C62" t="s">
-        <v>84</v>
+        <v>81</v>
+      </c>
+      <c r="D62" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="B64" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B66" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C66" t="s">
         <v>88</v>
       </c>
+      <c r="D66" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>89</v>
-      </c>
-      <c r="D67" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B68" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C68" t="s">
-        <v>89</v>
-      </c>
-      <c r="D68" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C69" t="s">
-        <v>92</v>
-      </c>
-      <c r="D69" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B70" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C70" t="s">
         <v>94</v>
@@ -1962,10 +2022,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C71" t="s">
         <v>95</v>
@@ -1973,10 +2033,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C72" t="s">
         <v>96</v>
@@ -1984,7 +2044,7 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B73" t="s">
         <v>97</v>
@@ -1998,32 +2058,38 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74" t="s">
         <v>97</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
+        <v>97</v>
+      </c>
+      <c r="D74" t="s">
         <v>99</v>
-      </c>
-      <c r="C74" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75" t="s">
         <v>97</v>
       </c>
-      <c r="B75" t="s">
-        <v>99</v>
-      </c>
       <c r="C75" t="s">
+        <v>100</v>
+      </c>
+      <c r="D75" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" t="s">
         <v>97</v>
-      </c>
-      <c r="B76" t="s">
-        <v>99</v>
       </c>
       <c r="C76" t="s">
         <v>102</v>
@@ -2031,10 +2097,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>87</v>
+      </c>
+      <c r="B77" t="s">
         <v>97</v>
-      </c>
-      <c r="B77" t="s">
-        <v>99</v>
       </c>
       <c r="C77" t="s">
         <v>103</v>
@@ -2042,10 +2108,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" t="s">
         <v>97</v>
-      </c>
-      <c r="B78" t="s">
-        <v>104</v>
       </c>
       <c r="C78" t="s">
         <v>104</v>
@@ -2053,124 +2119,112 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B79" t="s">
         <v>105</v>
       </c>
       <c r="C79" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B80" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C80" t="s">
-        <v>106</v>
-      </c>
-      <c r="D80" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B81" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C81" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D81" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B82" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C82" t="s">
-        <v>106</v>
-      </c>
-      <c r="D82" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B83" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C83" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B84" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C84" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B85" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C85" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B86" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C86" t="s">
-        <v>115</v>
-      </c>
-      <c r="D86" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B87" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C87" t="s">
-        <v>115</v>
-      </c>
-      <c r="D87" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B88" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C88" t="s">
         <v>118</v>
@@ -2181,10 +2235,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B89" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C89" t="s">
         <v>118</v>
@@ -2195,10 +2249,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B90" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C90" t="s">
         <v>118</v>
@@ -2209,35 +2263,29 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B91" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C91" t="s">
-        <v>118</v>
-      </c>
-      <c r="D91" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B92" t="s">
         <v>123</v>
       </c>
       <c r="C92" t="s">
-        <v>123</v>
-      </c>
-      <c r="D92" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B93" t="s">
         <v>123</v>
@@ -2248,10 +2296,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>118</v>
+      </c>
+      <c r="B94" t="s">
         <v>123</v>
-      </c>
-      <c r="B94" t="s">
-        <v>126</v>
       </c>
       <c r="C94" t="s">
         <v>126</v>
@@ -2259,163 +2307,160 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B95" t="s">
         <v>127</v>
       </c>
       <c r="C95" t="s">
-        <v>127</v>
+        <v>128</v>
+      </c>
+      <c r="D95" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B96" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C96" t="s">
         <v>128</v>
       </c>
+      <c r="D96" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B97" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C97" t="s">
         <v>131</v>
       </c>
+      <c r="D97" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B98" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C98" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="D98" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B99" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C99" t="s">
+        <v>131</v>
+      </c>
+      <c r="D99" t="s">
         <v>134</v>
-      </c>
-      <c r="D99" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B100" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C100" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D100" t="s">
-        <v>136</v>
-      </c>
-      <c r="E100" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B101" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C101" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D101" t="s">
-        <v>136</v>
-      </c>
-      <c r="E101" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B102" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C102" t="s">
-        <v>140</v>
-      </c>
-      <c r="D102" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B103" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C103" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B104" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C104" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B105" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C105" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>142</v>
       </c>
-      <c r="B106" t="s">
-        <v>146</v>
-      </c>
-      <c r="C106" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>142</v>
       </c>
       <c r="B107" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C107" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2423,10 +2468,10 @@
         <v>142</v>
       </c>
       <c r="B108" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C108" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2437,7 +2482,10 @@
         <v>146</v>
       </c>
       <c r="C109" t="s">
-        <v>150</v>
+        <v>147</v>
+      </c>
+      <c r="D109" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2448,7 +2496,13 @@
         <v>146</v>
       </c>
       <c r="C110" t="s">
-        <v>151</v>
+        <v>147</v>
+      </c>
+      <c r="D110" t="s">
+        <v>149</v>
+      </c>
+      <c r="E110" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2456,10 +2510,16 @@
         <v>142</v>
       </c>
       <c r="B111" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C111" t="s">
-        <v>153</v>
+        <v>147</v>
+      </c>
+      <c r="D111" t="s">
+        <v>149</v>
+      </c>
+      <c r="E111" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2470,10 +2530,10 @@
         <v>152</v>
       </c>
       <c r="C112" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>142</v>
       </c>
@@ -2481,318 +2541,487 @@
         <v>152</v>
       </c>
       <c r="C113" t="s">
-        <v>155</v>
-      </c>
-      <c r="D113" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>142</v>
       </c>
       <c r="B114" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C114" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D114" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>142</v>
       </c>
       <c r="B115" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C115" t="s">
-        <v>155</v>
-      </c>
-      <c r="D115" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>142</v>
       </c>
       <c r="B116" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C116" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>142</v>
+      </c>
+      <c r="B117" t="s">
         <v>155</v>
-      </c>
-      <c r="D116" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>160</v>
-      </c>
-      <c r="B117" t="s">
-        <v>160</v>
       </c>
       <c r="C117" t="s">
         <v>160</v>
       </c>
-      <c r="D117" t="s">
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>160</v>
-      </c>
       <c r="B118" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C118" t="s">
         <v>162</v>
       </c>
-      <c r="D118" t="s">
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>161</v>
+      </c>
+      <c r="B119" t="s">
+        <v>161</v>
+      </c>
+      <c r="C119" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>160</v>
-      </c>
-      <c r="B119" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>161</v>
+      </c>
+      <c r="B120" t="s">
+        <v>161</v>
+      </c>
+      <c r="C120" t="s">
         <v>164</v>
       </c>
-      <c r="C119" t="s">
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>161</v>
+      </c>
+      <c r="B121" t="s">
         <v>165</v>
       </c>
-      <c r="D119" t="s">
+      <c r="C121" t="s">
         <v>166</v>
       </c>
-      <c r="E119" t="s">
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>161</v>
+      </c>
+      <c r="B122" t="s">
+        <v>165</v>
+      </c>
+      <c r="C122" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>160</v>
-      </c>
-      <c r="B120" t="s">
-        <v>164</v>
-      </c>
-      <c r="C120" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>161</v>
+      </c>
+      <c r="B123" t="s">
         <v>165</v>
       </c>
-      <c r="D120" t="s">
+      <c r="C123" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>160</v>
-      </c>
-      <c r="B121" t="s">
-        <v>164</v>
-      </c>
-      <c r="C121" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>161</v>
+      </c>
+      <c r="B124" t="s">
         <v>165</v>
       </c>
-      <c r="D121" t="s">
+      <c r="C124" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>160</v>
-      </c>
-      <c r="B122" t="s">
-        <v>164</v>
-      </c>
-      <c r="C122" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>161</v>
+      </c>
+      <c r="B125" t="s">
         <v>165</v>
       </c>
-      <c r="D122" t="s">
+      <c r="C125" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>160</v>
-      </c>
-      <c r="B123" t="s">
-        <v>164</v>
-      </c>
-      <c r="C123" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>161</v>
+      </c>
+      <c r="B126" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>160</v>
-      </c>
-      <c r="B124" t="s">
-        <v>164</v>
-      </c>
-      <c r="C124" t="s">
+      <c r="C126" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>160</v>
-      </c>
-      <c r="B125" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>161</v>
+      </c>
+      <c r="B127" t="s">
+        <v>171</v>
+      </c>
+      <c r="C127" t="s">
         <v>173</v>
       </c>
-      <c r="C125" t="s">
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>161</v>
+      </c>
+      <c r="B128" t="s">
+        <v>171</v>
+      </c>
+      <c r="C128" t="s">
         <v>174</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D128" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>160</v>
-      </c>
-      <c r="B126" t="s">
-        <v>173</v>
-      </c>
-      <c r="C126" t="s">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>161</v>
+      </c>
+      <c r="B129" t="s">
+        <v>171</v>
+      </c>
+      <c r="C129" t="s">
         <v>174</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D129" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>160</v>
-      </c>
-      <c r="B127" t="s">
-        <v>173</v>
-      </c>
-      <c r="C127" t="s">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>161</v>
+      </c>
+      <c r="B130" t="s">
+        <v>171</v>
+      </c>
+      <c r="C130" t="s">
+        <v>174</v>
+      </c>
+      <c r="D130" t="s">
         <v>177</v>
       </c>
-      <c r="D127" t="s">
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>161</v>
+      </c>
+      <c r="B131" t="s">
+        <v>171</v>
+      </c>
+      <c r="C131" t="s">
+        <v>174</v>
+      </c>
+      <c r="D131" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>160</v>
-      </c>
-      <c r="B128" t="s">
-        <v>173</v>
-      </c>
-      <c r="C128" t="s">
-        <v>177</v>
-      </c>
-      <c r="D128" t="s">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>160</v>
-      </c>
-      <c r="B129" t="s">
-        <v>173</v>
-      </c>
-      <c r="C129" t="s">
-        <v>177</v>
-      </c>
-      <c r="D129" t="s">
+      <c r="B132" t="s">
+        <v>179</v>
+      </c>
+      <c r="C132" t="s">
+        <v>179</v>
+      </c>
+      <c r="D132" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>160</v>
-      </c>
-      <c r="B130" t="s">
-        <v>173</v>
-      </c>
-      <c r="C130" t="s">
-        <v>177</v>
-      </c>
-      <c r="D130" t="s">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>179</v>
+      </c>
+      <c r="B133" t="s">
+        <v>179</v>
+      </c>
+      <c r="C133" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>160</v>
-      </c>
-      <c r="B131" t="s">
-        <v>173</v>
-      </c>
-      <c r="C131" t="s">
-        <v>177</v>
-      </c>
-      <c r="D131" t="s">
+      <c r="D133" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>160</v>
-      </c>
-      <c r="B132" t="s">
-        <v>173</v>
-      </c>
-      <c r="C132" t="s">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>179</v>
+      </c>
+      <c r="B134" t="s">
         <v>183</v>
       </c>
-      <c r="D132" t="s">
+      <c r="C134" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>160</v>
-      </c>
-      <c r="B133" t="s">
-        <v>173</v>
-      </c>
-      <c r="C133" t="s">
+      <c r="D134" t="s">
+        <v>185</v>
+      </c>
+      <c r="E134" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>179</v>
+      </c>
+      <c r="B135" t="s">
         <v>183</v>
       </c>
-      <c r="D133" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>160</v>
-      </c>
-      <c r="B134" t="s">
-        <v>173</v>
-      </c>
-      <c r="C134" t="s">
-        <v>183</v>
-      </c>
-      <c r="D134" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>160</v>
-      </c>
-      <c r="B135" t="s">
-        <v>173</v>
-      </c>
       <c r="C135" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D135" t="s">
         <v>187</v>
       </c>
     </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>179</v>
+      </c>
+      <c r="B136" t="s">
+        <v>183</v>
+      </c>
+      <c r="C136" t="s">
+        <v>184</v>
+      </c>
+      <c r="D136" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>179</v>
+      </c>
+      <c r="B137" t="s">
+        <v>183</v>
+      </c>
+      <c r="C137" t="s">
+        <v>184</v>
+      </c>
+      <c r="D137" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>179</v>
+      </c>
+      <c r="B138" t="s">
+        <v>183</v>
+      </c>
+      <c r="C138" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>179</v>
+      </c>
+      <c r="B139" t="s">
+        <v>183</v>
+      </c>
+      <c r="C139" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>179</v>
+      </c>
+      <c r="B140" t="s">
+        <v>192</v>
+      </c>
+      <c r="C140" t="s">
+        <v>193</v>
+      </c>
+      <c r="D140" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>179</v>
+      </c>
+      <c r="B141" t="s">
+        <v>192</v>
+      </c>
+      <c r="C141" t="s">
+        <v>193</v>
+      </c>
+      <c r="D141" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>179</v>
+      </c>
+      <c r="B142" t="s">
+        <v>192</v>
+      </c>
+      <c r="C142" t="s">
+        <v>196</v>
+      </c>
+      <c r="D142" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>179</v>
+      </c>
+      <c r="B143" t="s">
+        <v>192</v>
+      </c>
+      <c r="C143" t="s">
+        <v>196</v>
+      </c>
+      <c r="D143" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>179</v>
+      </c>
+      <c r="B144" t="s">
+        <v>192</v>
+      </c>
+      <c r="C144" t="s">
+        <v>196</v>
+      </c>
+      <c r="D144" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>179</v>
+      </c>
+      <c r="B145" t="s">
+        <v>192</v>
+      </c>
+      <c r="C145" t="s">
+        <v>196</v>
+      </c>
+      <c r="D145" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>179</v>
+      </c>
+      <c r="B146" t="s">
+        <v>192</v>
+      </c>
+      <c r="C146" t="s">
+        <v>196</v>
+      </c>
+      <c r="D146" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>179</v>
+      </c>
+      <c r="B147" t="s">
+        <v>192</v>
+      </c>
+      <c r="C147" t="s">
+        <v>202</v>
+      </c>
+      <c r="D147" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>179</v>
+      </c>
+      <c r="B148" t="s">
+        <v>192</v>
+      </c>
+      <c r="C148" t="s">
+        <v>202</v>
+      </c>
+      <c r="D148" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>179</v>
+      </c>
+      <c r="B149" t="s">
+        <v>192</v>
+      </c>
+      <c r="C149" t="s">
+        <v>202</v>
+      </c>
+      <c r="D149" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>179</v>
+      </c>
+      <c r="B150" t="s">
+        <v>192</v>
+      </c>
+      <c r="C150" t="s">
+        <v>202</v>
+      </c>
+      <c r="D150" t="s">
+        <v>206</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>